<commit_message>
Changes for UI Design
Changes for UI Design
</commit_message>
<xml_diff>
--- a/01_Requirements/LedgerTypes/010_Loans ledger creation.xlsx
+++ b/01_Requirements/LedgerTypes/010_Loans ledger creation.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Loan Ledger'!$D$4:$D$39</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,9 +42,6 @@
     <t xml:space="preserve">Loan ( Secured/ Unsecured) ledgers Creation </t>
   </si>
   <si>
-    <t xml:space="preserve">Name of the Bank / Fin. Institution </t>
-  </si>
-  <si>
     <t xml:space="preserve">ABC &amp; Co </t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Bank Account no of the Loan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Loan amount remittance account </t>
   </si>
   <si>
@@ -151,13 +145,19 @@
   </si>
   <si>
     <t>Drop Down list of TDS Rates</t>
+  </si>
+  <si>
+    <t>Loan Account Name</t>
+  </si>
+  <si>
+    <t>Bank Account for Loan amount remittance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,26 +356,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -386,6 +371,84 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -395,71 +458,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -777,11 +777,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:J43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="E5:J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1"/>
   <cols>
     <col min="1" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="60.28515625" style="1" customWidth="1"/>
@@ -790,440 +790,447 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="4:10" ht="24.95" customHeight="1">
       <c r="D2" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="4:10" ht="24.95" customHeight="1" thickBot="1"/>
+    <row r="4" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="32"/>
-    </row>
-    <row r="5" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="5" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
       <c r="D5" s="2"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="34"/>
-    </row>
-    <row r="6" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="26"/>
+    </row>
+    <row r="6" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
       <c r="D6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="26"/>
+    </row>
+    <row r="7" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D7" s="2"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="26"/>
+    </row>
+    <row r="8" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="34"/>
-    </row>
-    <row r="7" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="2"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="34"/>
-    </row>
-    <row r="8" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="F8" s="17"/>
+      <c r="G8" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="12" t="s">
+      <c r="H8" s="17"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="26"/>
+    </row>
+    <row r="9" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D9" s="2"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="26"/>
+    </row>
+    <row r="10" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="34"/>
-    </row>
-    <row r="9" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="2"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="34"/>
-    </row>
-    <row r="10" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+    </row>
+    <row r="11" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D11" s="2"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="26"/>
+    </row>
+    <row r="12" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="34"/>
-    </row>
-    <row r="11" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="2"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="34"/>
-    </row>
-    <row r="12" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="34"/>
-    </row>
-    <row r="13" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="19"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="26"/>
+    </row>
+    <row r="13" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
       <c r="D13" s="2"/>
       <c r="E13" s="3"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="34"/>
-    </row>
-    <row r="14" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I13" s="25"/>
+      <c r="J13" s="26"/>
+    </row>
+    <row r="14" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
       <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="34"/>
-    </row>
-    <row r="15" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="26"/>
+    </row>
+    <row r="15" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="34"/>
-    </row>
-    <row r="16" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="25"/>
+      <c r="J15" s="26"/>
+    </row>
+    <row r="16" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
       <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
+    </row>
+    <row r="17" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D17" s="2"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="26"/>
+    </row>
+    <row r="18" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="34"/>
-    </row>
-    <row r="17" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="2"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34"/>
-    </row>
-    <row r="18" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D19" s="2"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="26"/>
+    </row>
+    <row r="20" spans="4:10" ht="38.450000000000003" customHeight="1" thickBot="1">
+      <c r="D20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="34"/>
-    </row>
-    <row r="19" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="2"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="33"/>
-      <c r="J19" s="34"/>
-    </row>
-    <row r="20" spans="4:10" ht="38.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="26"/>
+    </row>
+    <row r="21" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D21" s="2"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="26"/>
+    </row>
+    <row r="22" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="34"/>
-    </row>
-    <row r="21" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="2"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="34"/>
-    </row>
-    <row r="22" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="G22" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="H22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I22" s="33"/>
-      <c r="J22" s="34"/>
-    </row>
-    <row r="23" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="25"/>
+      <c r="J22" s="26"/>
+    </row>
+    <row r="23" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
       <c r="D23" s="2"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="34"/>
-    </row>
-    <row r="24" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="26"/>
+    </row>
+    <row r="24" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
       <c r="D24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="34"/>
-    </row>
-    <row r="25" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="26"/>
+    </row>
+    <row r="25" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
       <c r="D25" s="2"/>
       <c r="E25" s="3"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="34"/>
-    </row>
-    <row r="26" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I25" s="25"/>
+      <c r="J25" s="26"/>
+    </row>
+    <row r="26" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
       <c r="D26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="34"/>
-    </row>
-    <row r="27" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="26"/>
+    </row>
+    <row r="27" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
       <c r="D27" s="2"/>
       <c r="E27" s="3"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="34"/>
-    </row>
-    <row r="28" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I27" s="25"/>
+      <c r="J27" s="26"/>
+    </row>
+    <row r="28" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
       <c r="D28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="26"/>
+    </row>
+    <row r="29" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D29" s="2"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="26"/>
+    </row>
+    <row r="30" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D30" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E30" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="34"/>
-    </row>
-    <row r="29" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="2"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="34"/>
-    </row>
-    <row r="30" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="2" t="s">
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="26"/>
+    </row>
+    <row r="31" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D31" s="2"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="26"/>
+    </row>
+    <row r="32" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E32" s="19"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="26"/>
+    </row>
+    <row r="33" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D33" s="2"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="26"/>
+    </row>
+    <row r="34" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="34"/>
-    </row>
-    <row r="31" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="2"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="34"/>
-    </row>
-    <row r="32" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="2" t="s">
+      <c r="E34" s="19"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="26"/>
+    </row>
+    <row r="35" spans="4:10" ht="24.95" customHeight="1">
+      <c r="D35" s="2"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="26"/>
+    </row>
+    <row r="36" spans="4:10" ht="24.95" customHeight="1">
+      <c r="D36" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E32" s="8"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="34"/>
-    </row>
-    <row r="33" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="2"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="34"/>
-    </row>
-    <row r="34" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="2" t="s">
+      <c r="E36" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="33"/>
-      <c r="J34" s="34"/>
-    </row>
-    <row r="35" spans="4:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D35" s="2"/>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="34"/>
-    </row>
-    <row r="36" spans="4:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="2" t="s">
+      <c r="F36" s="42"/>
+      <c r="G36" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="H36" s="42"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="26"/>
+    </row>
+    <row r="37" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D37" s="2"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="26"/>
+    </row>
+    <row r="38" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="26"/>
+    </row>
+    <row r="39" spans="4:10" ht="24.95" customHeight="1">
+      <c r="D39" s="2"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="26"/>
+    </row>
+    <row r="40" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D40" s="2"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="26"/>
+    </row>
+    <row r="41" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D41" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11" t="s">
+      <c r="E41" s="16"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="28"/>
+      <c r="J41" s="29"/>
+    </row>
+    <row r="42" spans="4:10" ht="24.95" customHeight="1" thickBot="1"/>
+    <row r="43" spans="4:10" ht="24.95" customHeight="1" thickBot="1">
+      <c r="D43" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="34"/>
-    </row>
-    <row r="37" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="2"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="34"/>
-    </row>
-    <row r="38" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="34"/>
-    </row>
-    <row r="39" spans="4:10" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="2"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="33"/>
-      <c r="J39" s="34"/>
-    </row>
-    <row r="40" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="2"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="33"/>
-      <c r="J40" s="34"/>
-    </row>
-    <row r="41" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E41" s="12"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="35"/>
-      <c r="J41" s="36"/>
-    </row>
-    <row r="42" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="4:10" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="17"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E38:H38"/>
+    <mergeCell ref="E41:H41"/>
+    <mergeCell ref="E20:H20"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="E34:H34"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:H36"/>
     <mergeCell ref="D43:J43"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="E6:H6"/>
@@ -1240,13 +1247,6 @@
     <mergeCell ref="E28:H28"/>
     <mergeCell ref="E30:H30"/>
     <mergeCell ref="E32:H32"/>
-    <mergeCell ref="E20:H20"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="E34:H34"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="E38:H38"/>
-    <mergeCell ref="E41:H41"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.11811023622047245" right="0.31496062992125984" top="0.15748031496062992" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>